<commit_message>
refactor(examples): improve excel examples code structure
Restructure and enhance Excel-related example files with:
- Consistent code formatting and organization
- English documentation replacing Russian comments
- Standardized error handling with result checking
- Clearer example structure with numbered examples
- More descriptive variable naming
- Improved output messages for better understanding
</commit_message>
<xml_diff>
--- a/examples/System/XHEExcelFile/test/test.xlsx
+++ b/examples/System/XHEExcelFile/test/test.xlsx
@@ -16,7 +16,6 @@
     <x:sheet name="new sheet3" sheetId="6" r:id="rId7"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Новое имя111111111111111111112.'!$A$1:$B$200</x:definedName>
     <x:definedName name="Titles">Лист2!$C$1:$H$1</x:definedName>
   </x:definedNames>
   <x:calcPr refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
@@ -950,7 +949,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:28" ht="15" customHeight="1" hidden="1">
+    <x:row r="2" spans="1:28" ht="15" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -967,7 +966,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:28" ht="15" customHeight="1" hidden="1">
+    <x:row r="3" spans="1:28" ht="15" customHeight="1">
       <x:c r="A3" s="13" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1026,12 +1025,12 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:28" hidden="1">
+    <x:row r="4" spans="1:28">
       <x:c r="E4" s="23" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:28" hidden="1">
+    <x:row r="5" spans="1:28">
       <x:c r="B5" s="15">
         <x:v>65.2311212</x:v>
       </x:c>
@@ -1039,797 +1038,14 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:28" hidden="1">
+    <x:row r="6" spans="1:28">
       <x:c r="B6" s="15">
         <x:v>65.2311212</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:28" hidden="1">
-      <x:c r="B7" s="15"/>
-      <x:c r="M7" s="2"/>
-    </x:row>
-    <x:row r="8" spans="1:28" hidden="1">
-      <x:c r="B8" s="15"/>
-      <x:c r="M8" s="2"/>
-    </x:row>
-    <x:row r="9" spans="1:28" hidden="1">
-      <x:c r="B9" s="15"/>
-      <x:c r="M9" s="2"/>
-    </x:row>
-    <x:row r="10" spans="1:28" hidden="1">
-      <x:c r="B10" s="15"/>
-      <x:c r="M10" s="2"/>
-    </x:row>
-    <x:row r="11" spans="1:28" hidden="1">
-      <x:c r="B11" s="15"/>
-      <x:c r="M11" s="2"/>
-    </x:row>
-    <x:row r="12" spans="1:28" hidden="1">
-      <x:c r="B12" s="15"/>
-      <x:c r="M12" s="2"/>
-    </x:row>
-    <x:row r="13" spans="1:28" hidden="1">
-      <x:c r="B13" s="15"/>
-      <x:c r="M13" s="2"/>
-    </x:row>
-    <x:row r="14" spans="1:28" hidden="1">
-      <x:c r="B14" s="15"/>
-      <x:c r="M14" s="2"/>
-    </x:row>
-    <x:row r="15" spans="1:28" hidden="1">
-      <x:c r="B15" s="15"/>
-      <x:c r="M15" s="2"/>
-    </x:row>
-    <x:row r="16" spans="1:28" hidden="1">
-      <x:c r="B16" s="15"/>
-      <x:c r="M16" s="2"/>
-    </x:row>
-    <x:row r="17" spans="1:28" hidden="1">
-      <x:c r="B17" s="15"/>
-      <x:c r="M17" s="2"/>
-    </x:row>
-    <x:row r="18" spans="1:28" hidden="1">
-      <x:c r="B18" s="15"/>
-      <x:c r="M18" s="2"/>
-    </x:row>
-    <x:row r="19" spans="1:28" hidden="1">
-      <x:c r="B19" s="15"/>
-      <x:c r="M19" s="2"/>
-    </x:row>
-    <x:row r="20" spans="1:28" hidden="1">
-      <x:c r="B20" s="15"/>
-      <x:c r="M20" s="2"/>
-    </x:row>
-    <x:row r="21" spans="1:28" hidden="1">
-      <x:c r="B21" s="15"/>
-      <x:c r="M21" s="2"/>
-    </x:row>
-    <x:row r="22" spans="1:28" hidden="1">
-      <x:c r="B22" s="15"/>
-      <x:c r="M22" s="2"/>
-    </x:row>
-    <x:row r="23" spans="1:28" hidden="1">
-      <x:c r="B23" s="15"/>
-      <x:c r="M23" s="2"/>
-    </x:row>
-    <x:row r="24" spans="1:28" hidden="1">
-      <x:c r="B24" s="15"/>
-      <x:c r="M24" s="2"/>
-    </x:row>
-    <x:row r="25" spans="1:28" hidden="1">
-      <x:c r="B25" s="15"/>
-      <x:c r="M25" s="2"/>
-    </x:row>
-    <x:row r="26" spans="1:28" hidden="1">
-      <x:c r="B26" s="15"/>
-      <x:c r="M26" s="2"/>
-    </x:row>
-    <x:row r="27" spans="1:28" hidden="1">
-      <x:c r="B27" s="15"/>
-      <x:c r="M27" s="2"/>
-    </x:row>
-    <x:row r="28" spans="1:28" hidden="1">
-      <x:c r="B28" s="15"/>
-      <x:c r="M28" s="2"/>
-    </x:row>
-    <x:row r="29" spans="1:28" hidden="1">
-      <x:c r="B29" s="15"/>
-      <x:c r="M29" s="2"/>
-    </x:row>
-    <x:row r="30" spans="1:28" hidden="1">
-      <x:c r="B30" s="15"/>
-      <x:c r="M30" s="2"/>
-    </x:row>
-    <x:row r="31" spans="1:28" hidden="1">
-      <x:c r="B31" s="15"/>
-      <x:c r="M31" s="2"/>
-    </x:row>
-    <x:row r="32" spans="1:28" hidden="1">
-      <x:c r="B32" s="15"/>
-      <x:c r="M32" s="2"/>
-    </x:row>
-    <x:row r="33" spans="1:28" hidden="1">
-      <x:c r="B33" s="15"/>
-      <x:c r="M33" s="2"/>
-    </x:row>
-    <x:row r="34" spans="1:28" hidden="1">
-      <x:c r="B34" s="15"/>
-      <x:c r="M34" s="2"/>
-    </x:row>
-    <x:row r="35" spans="1:28" hidden="1">
-      <x:c r="B35" s="15"/>
-      <x:c r="M35" s="2"/>
-    </x:row>
-    <x:row r="36" spans="1:28" hidden="1">
-      <x:c r="B36" s="15"/>
-      <x:c r="M36" s="2"/>
-    </x:row>
-    <x:row r="37" spans="1:28" hidden="1">
-      <x:c r="B37" s="15"/>
-      <x:c r="M37" s="2"/>
-    </x:row>
-    <x:row r="38" spans="1:28" hidden="1">
-      <x:c r="B38" s="15"/>
-      <x:c r="M38" s="2"/>
-    </x:row>
-    <x:row r="39" spans="1:28" hidden="1">
-      <x:c r="B39" s="15"/>
-      <x:c r="M39" s="2"/>
-    </x:row>
-    <x:row r="40" spans="1:28" hidden="1">
-      <x:c r="B40" s="15"/>
-      <x:c r="M40" s="2"/>
-    </x:row>
-    <x:row r="41" spans="1:28" hidden="1">
-      <x:c r="B41" s="15"/>
-      <x:c r="M41" s="2"/>
-    </x:row>
-    <x:row r="42" spans="1:28" hidden="1">
-      <x:c r="B42" s="15"/>
-      <x:c r="M42" s="2"/>
-    </x:row>
-    <x:row r="43" spans="1:28" hidden="1">
-      <x:c r="B43" s="15"/>
-      <x:c r="M43" s="2"/>
-    </x:row>
-    <x:row r="44" spans="1:28" hidden="1">
-      <x:c r="B44" s="15"/>
-      <x:c r="M44" s="2"/>
-    </x:row>
-    <x:row r="45" spans="1:28" hidden="1">
-      <x:c r="B45" s="15"/>
-      <x:c r="M45" s="2"/>
-    </x:row>
-    <x:row r="46" spans="1:28" hidden="1">
-      <x:c r="B46" s="15"/>
-      <x:c r="M46" s="2"/>
-    </x:row>
-    <x:row r="47" spans="1:28" hidden="1">
-      <x:c r="B47" s="15"/>
-      <x:c r="M47" s="2"/>
-    </x:row>
-    <x:row r="48" spans="1:28" hidden="1">
-      <x:c r="B48" s="15"/>
-      <x:c r="M48" s="2"/>
-    </x:row>
-    <x:row r="49" spans="1:28" hidden="1">
-      <x:c r="B49" s="15"/>
-      <x:c r="M49" s="2"/>
-    </x:row>
-    <x:row r="50" spans="1:28" hidden="1">
-      <x:c r="B50" s="15"/>
-      <x:c r="M50" s="2"/>
-    </x:row>
-    <x:row r="51" spans="1:28" hidden="1">
-      <x:c r="B51" s="15"/>
-      <x:c r="M51" s="2"/>
-    </x:row>
-    <x:row r="52" spans="1:28" hidden="1">
-      <x:c r="B52" s="15"/>
-      <x:c r="M52" s="2"/>
-    </x:row>
-    <x:row r="53" spans="1:28" hidden="1">
-      <x:c r="B53" s="15"/>
-      <x:c r="M53" s="2"/>
-    </x:row>
-    <x:row r="54" spans="1:28" hidden="1">
-      <x:c r="B54" s="15"/>
-      <x:c r="M54" s="2"/>
-    </x:row>
-    <x:row r="55" spans="1:28" hidden="1">
-      <x:c r="B55" s="15"/>
-      <x:c r="M55" s="2"/>
-    </x:row>
-    <x:row r="56" spans="1:28" hidden="1">
-      <x:c r="B56" s="15"/>
-      <x:c r="M56" s="2"/>
-    </x:row>
-    <x:row r="57" spans="1:28" hidden="1">
-      <x:c r="B57" s="15"/>
-      <x:c r="M57" s="2"/>
-    </x:row>
-    <x:row r="58" spans="1:28" hidden="1">
-      <x:c r="B58" s="15"/>
-      <x:c r="M58" s="2"/>
-    </x:row>
-    <x:row r="59" spans="1:28" hidden="1">
-      <x:c r="B59" s="15"/>
-      <x:c r="M59" s="2"/>
-    </x:row>
-    <x:row r="60" spans="1:28" hidden="1">
-      <x:c r="B60" s="15"/>
-      <x:c r="M60" s="2"/>
-    </x:row>
-    <x:row r="61" spans="1:28" hidden="1">
-      <x:c r="B61" s="15"/>
-      <x:c r="M61" s="2"/>
-    </x:row>
-    <x:row r="62" spans="1:28" hidden="1">
-      <x:c r="B62" s="15"/>
-      <x:c r="M62" s="2"/>
-    </x:row>
-    <x:row r="63" spans="1:28" hidden="1">
-      <x:c r="B63" s="15"/>
-      <x:c r="M63" s="2"/>
-    </x:row>
-    <x:row r="64" spans="1:28" hidden="1">
-      <x:c r="B64" s="15"/>
-      <x:c r="M64" s="2"/>
-    </x:row>
-    <x:row r="65" spans="1:28" hidden="1">
-      <x:c r="B65" s="15"/>
-      <x:c r="M65" s="2"/>
-    </x:row>
-    <x:row r="66" spans="1:28" hidden="1">
-      <x:c r="B66" s="15"/>
-      <x:c r="M66" s="2"/>
-    </x:row>
-    <x:row r="67" spans="1:28" hidden="1">
-      <x:c r="B67" s="15"/>
-      <x:c r="M67" s="2"/>
-    </x:row>
-    <x:row r="68" spans="1:28" hidden="1">
-      <x:c r="B68" s="15"/>
-      <x:c r="M68" s="2"/>
-    </x:row>
-    <x:row r="69" spans="1:28" hidden="1">
-      <x:c r="B69" s="15"/>
-      <x:c r="M69" s="2"/>
-    </x:row>
-    <x:row r="70" spans="1:28" hidden="1">
-      <x:c r="B70" s="15"/>
-      <x:c r="M70" s="2"/>
-    </x:row>
-    <x:row r="71" spans="1:28" hidden="1">
-      <x:c r="B71" s="15"/>
-      <x:c r="M71" s="2"/>
-    </x:row>
-    <x:row r="72" spans="1:28" hidden="1">
-      <x:c r="B72" s="15"/>
-      <x:c r="M72" s="2"/>
-    </x:row>
-    <x:row r="73" spans="1:28" hidden="1">
-      <x:c r="B73" s="15"/>
-      <x:c r="M73" s="2"/>
-    </x:row>
-    <x:row r="74" spans="1:28" hidden="1">
-      <x:c r="B74" s="15"/>
-      <x:c r="M74" s="2"/>
-    </x:row>
-    <x:row r="75" spans="1:28" hidden="1">
-      <x:c r="B75" s="15"/>
-      <x:c r="M75" s="2"/>
-    </x:row>
-    <x:row r="76" spans="1:28" hidden="1">
-      <x:c r="B76" s="15"/>
-      <x:c r="M76" s="2"/>
-    </x:row>
-    <x:row r="77" spans="1:28" hidden="1">
-      <x:c r="B77" s="15"/>
-      <x:c r="M77" s="2"/>
-    </x:row>
-    <x:row r="78" spans="1:28" hidden="1">
-      <x:c r="B78" s="15"/>
-      <x:c r="M78" s="2"/>
-    </x:row>
-    <x:row r="79" spans="1:28" hidden="1">
-      <x:c r="B79" s="15"/>
-      <x:c r="M79" s="2"/>
-    </x:row>
-    <x:row r="80" spans="1:28" hidden="1">
-      <x:c r="B80" s="15"/>
-      <x:c r="M80" s="2"/>
-    </x:row>
-    <x:row r="81" spans="1:28" hidden="1">
-      <x:c r="B81" s="15"/>
-      <x:c r="M81" s="2"/>
-    </x:row>
-    <x:row r="82" spans="1:28" hidden="1">
-      <x:c r="B82" s="15"/>
-      <x:c r="M82" s="2"/>
-    </x:row>
-    <x:row r="83" spans="1:28" hidden="1">
-      <x:c r="B83" s="15"/>
-      <x:c r="M83" s="2"/>
-    </x:row>
-    <x:row r="84" spans="1:28" hidden="1">
-      <x:c r="B84" s="15"/>
-      <x:c r="M84" s="2"/>
-    </x:row>
-    <x:row r="85" spans="1:28" hidden="1">
-      <x:c r="B85" s="15"/>
-      <x:c r="M85" s="2"/>
-    </x:row>
-    <x:row r="86" spans="1:28" hidden="1">
-      <x:c r="B86" s="15"/>
-      <x:c r="M86" s="2"/>
-    </x:row>
-    <x:row r="87" spans="1:28" hidden="1">
-      <x:c r="B87" s="15"/>
-      <x:c r="M87" s="2"/>
-    </x:row>
-    <x:row r="88" spans="1:28" hidden="1">
-      <x:c r="B88" s="15"/>
-      <x:c r="M88" s="2"/>
-    </x:row>
-    <x:row r="89" spans="1:28" hidden="1">
-      <x:c r="B89" s="15"/>
-      <x:c r="M89" s="2"/>
-    </x:row>
-    <x:row r="90" spans="1:28" hidden="1">
-      <x:c r="B90" s="15"/>
-      <x:c r="M90" s="2"/>
-    </x:row>
-    <x:row r="91" spans="1:28" hidden="1">
-      <x:c r="B91" s="15"/>
-      <x:c r="M91" s="2"/>
-    </x:row>
-    <x:row r="92" spans="1:28" hidden="1">
-      <x:c r="B92" s="15"/>
-      <x:c r="M92" s="2"/>
-    </x:row>
-    <x:row r="93" spans="1:28" hidden="1">
-      <x:c r="B93" s="15"/>
-      <x:c r="M93" s="2"/>
-    </x:row>
-    <x:row r="94" spans="1:28" hidden="1">
-      <x:c r="B94" s="15"/>
-      <x:c r="M94" s="2"/>
-    </x:row>
-    <x:row r="95" spans="1:28" hidden="1">
-      <x:c r="B95" s="15"/>
-      <x:c r="M95" s="2"/>
-    </x:row>
-    <x:row r="96" spans="1:28" hidden="1">
-      <x:c r="B96" s="15"/>
-      <x:c r="M96" s="2"/>
-    </x:row>
-    <x:row r="97" spans="1:28" hidden="1">
-      <x:c r="B97" s="15"/>
-      <x:c r="M97" s="2"/>
-    </x:row>
-    <x:row r="98" spans="1:28" hidden="1">
-      <x:c r="B98" s="15"/>
-      <x:c r="M98" s="2"/>
-    </x:row>
-    <x:row r="99" spans="1:28" hidden="1">
-      <x:c r="B99" s="15"/>
-      <x:c r="M99" s="2"/>
-    </x:row>
-    <x:row r="100" spans="1:28" hidden="1">
-      <x:c r="B100" s="15"/>
-      <x:c r="M100" s="2"/>
-    </x:row>
-    <x:row r="101" spans="1:28" hidden="1">
-      <x:c r="B101" s="15"/>
-      <x:c r="M101" s="2"/>
-    </x:row>
-    <x:row r="102" spans="1:28" hidden="1">
-      <x:c r="B102" s="15"/>
-      <x:c r="M102" s="2"/>
-    </x:row>
-    <x:row r="103" spans="1:28" hidden="1">
-      <x:c r="B103" s="15"/>
-      <x:c r="M103" s="2"/>
-    </x:row>
-    <x:row r="104" spans="1:28" hidden="1">
-      <x:c r="B104" s="15"/>
-      <x:c r="M104" s="2"/>
-    </x:row>
-    <x:row r="105" spans="1:28" hidden="1">
-      <x:c r="B105" s="15"/>
-      <x:c r="M105" s="2"/>
-    </x:row>
-    <x:row r="106" spans="1:28" hidden="1">
-      <x:c r="B106" s="15"/>
-      <x:c r="M106" s="2"/>
-    </x:row>
-    <x:row r="107" spans="1:28" hidden="1">
-      <x:c r="B107" s="15"/>
-      <x:c r="M107" s="2"/>
-    </x:row>
-    <x:row r="108" spans="1:28" hidden="1">
-      <x:c r="B108" s="15"/>
-      <x:c r="M108" s="2"/>
-    </x:row>
-    <x:row r="109" spans="1:28" hidden="1">
-      <x:c r="B109" s="15"/>
-      <x:c r="M109" s="2"/>
-    </x:row>
-    <x:row r="110" spans="1:28" hidden="1">
-      <x:c r="B110" s="15"/>
-      <x:c r="M110" s="2"/>
-    </x:row>
-    <x:row r="111" spans="1:28" hidden="1">
-      <x:c r="B111" s="15"/>
-      <x:c r="M111" s="2"/>
-    </x:row>
-    <x:row r="112" spans="1:28" hidden="1">
-      <x:c r="B112" s="15"/>
-      <x:c r="M112" s="2"/>
-    </x:row>
-    <x:row r="113" spans="1:28" hidden="1">
-      <x:c r="B113" s="15"/>
-      <x:c r="M113" s="2"/>
-    </x:row>
-    <x:row r="114" spans="1:28" hidden="1">
-      <x:c r="B114" s="15"/>
-      <x:c r="M114" s="2"/>
-    </x:row>
-    <x:row r="115" spans="1:28" hidden="1">
-      <x:c r="B115" s="15"/>
-      <x:c r="M115" s="2"/>
-    </x:row>
-    <x:row r="116" spans="1:28" hidden="1">
-      <x:c r="B116" s="15"/>
-      <x:c r="M116" s="2"/>
-    </x:row>
-    <x:row r="117" spans="1:28" hidden="1">
-      <x:c r="B117" s="15"/>
-      <x:c r="M117" s="2"/>
-    </x:row>
-    <x:row r="118" spans="1:28" hidden="1">
-      <x:c r="B118" s="15"/>
-      <x:c r="M118" s="2"/>
-    </x:row>
-    <x:row r="119" spans="1:28" hidden="1">
-      <x:c r="B119" s="15"/>
-      <x:c r="M119" s="2"/>
-    </x:row>
-    <x:row r="120" spans="1:28" hidden="1">
-      <x:c r="B120" s="15"/>
-      <x:c r="M120" s="2"/>
-    </x:row>
-    <x:row r="121" spans="1:28" hidden="1">
-      <x:c r="B121" s="15"/>
-      <x:c r="M121" s="2"/>
-    </x:row>
-    <x:row r="122" spans="1:28" hidden="1">
-      <x:c r="B122" s="15"/>
-      <x:c r="M122" s="2"/>
-    </x:row>
-    <x:row r="123" spans="1:28" hidden="1">
-      <x:c r="B123" s="15"/>
-      <x:c r="M123" s="2"/>
-    </x:row>
-    <x:row r="124" spans="1:28" hidden="1">
-      <x:c r="B124" s="15"/>
-      <x:c r="M124" s="2"/>
-    </x:row>
-    <x:row r="125" spans="1:28" hidden="1">
-      <x:c r="B125" s="15"/>
-      <x:c r="M125" s="2"/>
-    </x:row>
-    <x:row r="126" spans="1:28" hidden="1">
-      <x:c r="B126" s="15"/>
-      <x:c r="M126" s="2"/>
-    </x:row>
-    <x:row r="127" spans="1:28" hidden="1">
-      <x:c r="B127" s="15"/>
-      <x:c r="M127" s="2"/>
-    </x:row>
-    <x:row r="128" spans="1:28" hidden="1">
-      <x:c r="B128" s="15"/>
-      <x:c r="M128" s="2"/>
-    </x:row>
-    <x:row r="129" spans="1:28" hidden="1">
-      <x:c r="B129" s="15"/>
-      <x:c r="M129" s="2"/>
-    </x:row>
-    <x:row r="130" spans="1:28" hidden="1">
-      <x:c r="B130" s="15"/>
-      <x:c r="M130" s="2"/>
-    </x:row>
-    <x:row r="131" spans="1:28" hidden="1">
-      <x:c r="B131" s="15"/>
-      <x:c r="M131" s="2"/>
-    </x:row>
-    <x:row r="132" spans="1:28" hidden="1">
-      <x:c r="B132" s="15"/>
-      <x:c r="M132" s="2"/>
-    </x:row>
-    <x:row r="133" spans="1:28" hidden="1">
-      <x:c r="B133" s="15"/>
-      <x:c r="M133" s="2"/>
-    </x:row>
-    <x:row r="134" spans="1:28" hidden="1">
-      <x:c r="B134" s="15"/>
-      <x:c r="M134" s="2"/>
-    </x:row>
-    <x:row r="135" spans="1:28" hidden="1">
-      <x:c r="B135" s="15"/>
-      <x:c r="M135" s="2"/>
-    </x:row>
-    <x:row r="136" spans="1:28" hidden="1">
-      <x:c r="B136" s="15"/>
-      <x:c r="M136" s="2"/>
-    </x:row>
-    <x:row r="137" spans="1:28" hidden="1">
-      <x:c r="B137" s="15"/>
-      <x:c r="M137" s="2"/>
-    </x:row>
-    <x:row r="138" spans="1:28" hidden="1">
-      <x:c r="B138" s="15"/>
-      <x:c r="M138" s="2"/>
-    </x:row>
-    <x:row r="139" spans="1:28" hidden="1">
-      <x:c r="B139" s="15"/>
-      <x:c r="M139" s="2"/>
-    </x:row>
-    <x:row r="140" spans="1:28" hidden="1">
-      <x:c r="B140" s="15"/>
-      <x:c r="M140" s="2"/>
-    </x:row>
-    <x:row r="141" spans="1:28" hidden="1">
-      <x:c r="B141" s="15"/>
-      <x:c r="M141" s="2"/>
-    </x:row>
-    <x:row r="142" spans="1:28" hidden="1">
-      <x:c r="B142" s="15"/>
-      <x:c r="M142" s="2"/>
-    </x:row>
-    <x:row r="143" spans="1:28" hidden="1">
-      <x:c r="B143" s="15"/>
-      <x:c r="M143" s="2"/>
-    </x:row>
-    <x:row r="144" spans="1:28" hidden="1">
-      <x:c r="B144" s="15"/>
-      <x:c r="M144" s="2"/>
-    </x:row>
-    <x:row r="145" spans="1:28" hidden="1">
-      <x:c r="B145" s="15"/>
-      <x:c r="M145" s="2"/>
-    </x:row>
-    <x:row r="146" spans="1:28" hidden="1">
-      <x:c r="B146" s="15"/>
-      <x:c r="M146" s="2"/>
-    </x:row>
-    <x:row r="147" spans="1:28" hidden="1">
-      <x:c r="B147" s="15"/>
-      <x:c r="M147" s="2"/>
-    </x:row>
-    <x:row r="148" spans="1:28" hidden="1">
-      <x:c r="B148" s="15"/>
-      <x:c r="M148" s="2"/>
-    </x:row>
-    <x:row r="149" spans="1:28" hidden="1">
-      <x:c r="B149" s="15"/>
-      <x:c r="M149" s="2"/>
-    </x:row>
-    <x:row r="150" spans="1:28" hidden="1">
-      <x:c r="B150" s="15"/>
-      <x:c r="M150" s="2"/>
-    </x:row>
-    <x:row r="151" spans="1:28" hidden="1">
-      <x:c r="B151" s="15"/>
-      <x:c r="M151" s="2"/>
-    </x:row>
-    <x:row r="152" spans="1:28" hidden="1">
-      <x:c r="B152" s="15"/>
-      <x:c r="M152" s="2"/>
-    </x:row>
-    <x:row r="153" spans="1:28" hidden="1">
-      <x:c r="B153" s="15"/>
-      <x:c r="M153" s="2"/>
-    </x:row>
-    <x:row r="154" spans="1:28" hidden="1">
-      <x:c r="B154" s="15"/>
-      <x:c r="M154" s="2"/>
-    </x:row>
-    <x:row r="155" spans="1:28" hidden="1">
-      <x:c r="B155" s="15"/>
-      <x:c r="M155" s="2"/>
-    </x:row>
-    <x:row r="156" spans="1:28" hidden="1">
-      <x:c r="B156" s="15"/>
-      <x:c r="M156" s="2"/>
-    </x:row>
-    <x:row r="157" spans="1:28" hidden="1">
-      <x:c r="B157" s="15"/>
-      <x:c r="M157" s="2"/>
-    </x:row>
-    <x:row r="158" spans="1:28" hidden="1">
-      <x:c r="B158" s="15"/>
-      <x:c r="M158" s="2"/>
-    </x:row>
-    <x:row r="159" spans="1:28" hidden="1">
-      <x:c r="B159" s="15"/>
-      <x:c r="M159" s="2"/>
-    </x:row>
-    <x:row r="160" spans="1:28" hidden="1">
-      <x:c r="B160" s="15"/>
-      <x:c r="M160" s="2"/>
-    </x:row>
-    <x:row r="161" spans="1:28" hidden="1">
-      <x:c r="B161" s="15"/>
-      <x:c r="M161" s="2"/>
-    </x:row>
-    <x:row r="162" spans="1:28" hidden="1">
-      <x:c r="B162" s="15"/>
-      <x:c r="M162" s="2"/>
-    </x:row>
-    <x:row r="163" spans="1:28" hidden="1">
-      <x:c r="B163" s="15"/>
-      <x:c r="M163" s="2"/>
-    </x:row>
-    <x:row r="164" spans="1:28" hidden="1">
-      <x:c r="B164" s="15"/>
-      <x:c r="M164" s="2"/>
-    </x:row>
-    <x:row r="165" spans="1:28" hidden="1">
-      <x:c r="B165" s="15"/>
-      <x:c r="M165" s="2"/>
-    </x:row>
-    <x:row r="166" spans="1:28" hidden="1">
-      <x:c r="B166" s="15"/>
-      <x:c r="M166" s="2"/>
-    </x:row>
-    <x:row r="167" spans="1:28" hidden="1">
-      <x:c r="B167" s="15"/>
-      <x:c r="M167" s="2"/>
-    </x:row>
-    <x:row r="168" spans="1:28" hidden="1">
-      <x:c r="B168" s="15"/>
-      <x:c r="M168" s="2"/>
-    </x:row>
-    <x:row r="169" spans="1:28" hidden="1">
-      <x:c r="B169" s="15"/>
-      <x:c r="M169" s="2"/>
-    </x:row>
-    <x:row r="170" spans="1:28" hidden="1">
-      <x:c r="B170" s="15"/>
-      <x:c r="M170" s="2"/>
-    </x:row>
-    <x:row r="171" spans="1:28" hidden="1">
-      <x:c r="B171" s="15"/>
-      <x:c r="M171" s="2"/>
-    </x:row>
-    <x:row r="172" spans="1:28" hidden="1">
-      <x:c r="B172" s="15"/>
-      <x:c r="M172" s="2"/>
-    </x:row>
-    <x:row r="173" spans="1:28" hidden="1">
-      <x:c r="B173" s="15"/>
-      <x:c r="M173" s="2"/>
-    </x:row>
-    <x:row r="174" spans="1:28" hidden="1">
-      <x:c r="B174" s="15"/>
-      <x:c r="M174" s="2"/>
-    </x:row>
-    <x:row r="175" spans="1:28" hidden="1">
-      <x:c r="B175" s="15"/>
-      <x:c r="M175" s="2"/>
-    </x:row>
-    <x:row r="176" spans="1:28" hidden="1">
-      <x:c r="B176" s="15"/>
-      <x:c r="M176" s="2"/>
-    </x:row>
-    <x:row r="177" spans="1:28" hidden="1">
-      <x:c r="B177" s="15"/>
-      <x:c r="M177" s="2"/>
-    </x:row>
-    <x:row r="178" spans="1:28" hidden="1">
-      <x:c r="B178" s="15"/>
-      <x:c r="M178" s="2"/>
-    </x:row>
-    <x:row r="179" spans="1:28" hidden="1">
-      <x:c r="B179" s="15"/>
-      <x:c r="M179" s="2"/>
-    </x:row>
-    <x:row r="180" spans="1:28" hidden="1">
-      <x:c r="B180" s="15"/>
-      <x:c r="M180" s="2"/>
-    </x:row>
-    <x:row r="181" spans="1:28" hidden="1">
-      <x:c r="B181" s="15"/>
-      <x:c r="M181" s="2"/>
-    </x:row>
-    <x:row r="182" spans="1:28" hidden="1">
-      <x:c r="B182" s="15"/>
-      <x:c r="M182" s="2"/>
-    </x:row>
-    <x:row r="183" spans="1:28" hidden="1">
-      <x:c r="B183" s="15"/>
-      <x:c r="M183" s="2"/>
-    </x:row>
-    <x:row r="184" spans="1:28" hidden="1">
-      <x:c r="B184" s="15"/>
-      <x:c r="M184" s="2"/>
-    </x:row>
-    <x:row r="185" spans="1:28" hidden="1">
-      <x:c r="B185" s="15"/>
-      <x:c r="M185" s="2"/>
-    </x:row>
-    <x:row r="186" spans="1:28" hidden="1">
-      <x:c r="B186" s="15"/>
-      <x:c r="M186" s="2"/>
-    </x:row>
-    <x:row r="187" spans="1:28" hidden="1">
-      <x:c r="B187" s="15"/>
-      <x:c r="M187" s="2"/>
-    </x:row>
-    <x:row r="188" spans="1:28" hidden="1">
-      <x:c r="B188" s="15"/>
-      <x:c r="M188" s="2"/>
-    </x:row>
-    <x:row r="189" spans="1:28" hidden="1">
-      <x:c r="B189" s="15"/>
-      <x:c r="M189" s="2"/>
-    </x:row>
-    <x:row r="190" spans="1:28" hidden="1">
-      <x:c r="B190" s="15"/>
-      <x:c r="M190" s="2"/>
-    </x:row>
-    <x:row r="191" spans="1:28" hidden="1">
-      <x:c r="B191" s="15"/>
-      <x:c r="M191" s="2"/>
-    </x:row>
-    <x:row r="192" spans="1:28" hidden="1">
-      <x:c r="B192" s="15"/>
-      <x:c r="M192" s="2"/>
-    </x:row>
-    <x:row r="193" spans="1:28" hidden="1">
-      <x:c r="B193" s="15"/>
-      <x:c r="M193" s="2"/>
-    </x:row>
-    <x:row r="194" spans="1:28" hidden="1">
-      <x:c r="B194" s="15"/>
-      <x:c r="M194" s="2"/>
-    </x:row>
-    <x:row r="195" spans="1:28" hidden="1">
-      <x:c r="B195" s="15"/>
-      <x:c r="M195" s="2"/>
-    </x:row>
-    <x:row r="196" spans="1:28" hidden="1">
-      <x:c r="B196" s="15"/>
-      <x:c r="M196" s="2"/>
-    </x:row>
-    <x:row r="197" spans="1:28" hidden="1">
-      <x:c r="B197" s="15"/>
-      <x:c r="M197" s="2"/>
-    </x:row>
-    <x:row r="198" spans="1:28" hidden="1">
-      <x:c r="B198" s="15"/>
-      <x:c r="M198" s="2"/>
-    </x:row>
-    <x:row r="199" spans="1:28" hidden="1">
-      <x:c r="B199" s="15"/>
-      <x:c r="M199" s="2"/>
-    </x:row>
-    <x:row r="200" spans="1:28" hidden="1">
-      <x:c r="B200" s="15"/>
-      <x:c r="M200" s="2"/>
-    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:B200">
-    <x:filterColumn colId="0">
-      <x:customFilters>
-        <x:customFilter val="1"/>
-      </x:customFilters>
-    </x:filterColumn>
-  </x:autoFilter>
   <x:hyperlinks>
-    <x:hyperlink ref="L1" r:id="rId13"/>
+    <x:hyperlink ref="L1" r:id="rId12"/>
     <x:hyperlink ref="L3" location="'new sheet'!A1" display="new sheet"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="true"/>

</xml_diff>